<commit_message>
Enviar mensagens no WhatsApp, pegando contatos da tabela no excel.
</commit_message>
<xml_diff>
--- a/Enviar.xlsx
+++ b/Enviar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b947908ecc1611d/Área de Trabalho/Wesley/python/MeusProjetos/automaçãowhats/WhatsApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{C2155F9C-95B5-40AE-82A0-3196F389692B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33A18780-2505-40EC-B62E-47D9E53C3D05}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{71860B2E-A64D-42A5-9A42-999386A06AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{F81C85CE-3BCD-4B33-8C8B-0A39913C8743}"/>
+    <workbookView xWindow="3495" yWindow="2010" windowWidth="15375" windowHeight="8325" xr2:uid="{A4DE314B-E9FB-46E2-AB97-BF98EDEA0F91}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Pessoa</t>
   </si>
@@ -43,28 +43,19 @@
     <t>Mensagem</t>
   </si>
   <si>
-    <t xml:space="preserve">aline </t>
-  </si>
-  <si>
-    <t xml:space="preserve">wagner </t>
-  </si>
-  <si>
-    <t>vanilza</t>
-  </si>
-  <si>
-    <t>oie, tudo bem ?</t>
-  </si>
-  <si>
     <t>teste</t>
   </si>
   <si>
-    <t>5511960435082</t>
-  </si>
-  <si>
-    <t>5511987813007</t>
-  </si>
-  <si>
-    <t>5511987676979</t>
+    <t>0000000000000</t>
+  </si>
+  <si>
+    <t>wesley</t>
+  </si>
+  <si>
+    <t>silva</t>
+  </si>
+  <si>
+    <t>almeida</t>
   </si>
 </sst>
 </file>
@@ -416,17 +407,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D53A7C94-CFFA-47EA-8C25-089A72CB0D85}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C55253-CFD5-4F66-9002-C10C1F9587A4}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -441,35 +429,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>